<commit_message>
New models for optimization and sensitivity
</commit_message>
<xml_diff>
--- a/Models/Model_final_matingao/ModelData.xlsx
+++ b/Models/Model_final_matingao/ModelData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714" firstSheet="2" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="714"/>
   </bookViews>
   <sheets>
     <sheet name="Dir" sheetId="5" r:id="rId1"/>
@@ -638,7 +638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -707,7 +707,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2550,8 +2550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>